<commit_message>
Subida inicial del código
</commit_message>
<xml_diff>
--- a/Temp/PlantillaCarga.xlsx
+++ b/Temp/PlantillaCarga.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.rodriguez\OneDrive - VIVA - EMPRESA DE VIVIENDA DE ANTIOQUIA\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vivagov-my.sharepoint.com/personal/daniel_rodriguez_viva_gov_co/Documents/Escritorio/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_B9BB2505A4397D6A206102B52094BE43A02C409B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BE8D671-AAAD-413E-9976-C3F0A696BA2E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CargaMasiva" sheetId="1" r:id="rId1"/>
@@ -402,7 +403,7 @@
     <t>ZARAGOZA</t>
   </si>
   <si>
-    <t xml:space="preserve">Ladrillo rojo de  3 x3 </t>
+    <t>Tornillos AA</t>
   </si>
   <si>
     <t>und</t>
@@ -411,7 +412,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -442,7 +443,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -781,11 +782,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DW2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,13 +1182,10 @@
         <v>128</v>
       </c>
       <c r="C2">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D2">
-        <v>124</v>
-      </c>
-      <c r="S2">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>